<commit_message>
Add stability check, reports, gain/loss by project graph, and input format documentation
</commit_message>
<xml_diff>
--- a/graficos/resultado_final.xlsx
+++ b/graficos/resultado_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>Rank Escolha</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Rank no Projeto</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Ganho/Perda</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +484,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +514,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +544,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +574,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +604,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +634,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,6 +664,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -614,6 +694,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -634,6 +724,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -654,6 +754,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -674,6 +784,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -694,6 +814,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -714,6 +844,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -734,6 +874,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -754,6 +904,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -774,6 +934,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -794,6 +964,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -814,6 +994,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -834,6 +1024,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -854,6 +1054,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -874,6 +1084,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -894,6 +1114,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -914,6 +1144,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -934,6 +1174,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -954,6 +1204,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -974,6 +1234,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -994,6 +1264,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1014,6 +1294,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1034,6 +1324,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1054,6 +1354,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1074,6 +1384,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1094,6 +1414,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1114,6 +1444,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1134,6 +1474,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1154,6 +1504,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1174,6 +1534,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1194,6 +1564,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1214,6 +1594,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1234,6 +1624,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1254,6 +1654,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1274,6 +1684,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1294,6 +1714,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1314,6 +1744,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1334,6 +1774,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1354,6 +1804,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1374,6 +1834,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1394,6 +1864,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1414,6 +1894,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1434,6 +1924,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1454,6 +1954,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>5ª</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1474,6 +1984,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1494,6 +2014,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1514,6 +2044,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1534,6 +2074,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1554,6 +2104,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1574,6 +2134,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1594,6 +2164,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1614,6 +2194,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1634,6 +2224,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1654,6 +2254,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1674,6 +2284,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1694,6 +2314,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1714,6 +2344,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1734,6 +2374,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1754,6 +2404,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1774,6 +2434,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1794,6 +2464,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1814,6 +2494,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1834,6 +2524,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1854,6 +2554,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1874,6 +2584,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1894,6 +2614,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1914,6 +2644,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1934,6 +2674,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1954,6 +2704,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1974,6 +2734,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1994,6 +2764,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2014,6 +2794,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2034,6 +2824,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2054,6 +2854,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2074,6 +2884,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2094,6 +2914,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>5ª</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2114,6 +2944,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>6ª</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2134,6 +2974,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2154,6 +3004,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2174,6 +3034,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2194,6 +3064,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2214,6 +3094,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2234,6 +3124,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2254,6 +3154,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2274,6 +3184,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2294,6 +3214,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2314,6 +3244,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2334,6 +3274,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2354,6 +3304,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2374,6 +3334,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2394,6 +3364,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2414,6 +3394,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2434,6 +3424,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2454,6 +3454,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2474,6 +3484,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2494,6 +3514,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2514,6 +3544,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2534,6 +3574,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2554,6 +3604,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2574,6 +3634,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2594,6 +3664,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2614,6 +3694,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2634,6 +3724,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2654,6 +3754,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>8ª</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2674,6 +3784,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2694,6 +3814,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2714,6 +3844,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2734,6 +3874,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2754,6 +3904,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2774,6 +3934,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2794,6 +3964,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2814,6 +3994,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2834,6 +4024,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2854,6 +4054,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2874,6 +4084,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2894,6 +4114,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2914,6 +4144,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2934,6 +4174,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2954,6 +4204,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2974,6 +4234,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2994,6 +4264,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3014,6 +4294,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3034,6 +4324,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3054,6 +4354,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3074,6 +4384,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3094,6 +4414,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3114,6 +4444,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3134,6 +4474,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3154,6 +4504,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>6ª</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3174,6 +4534,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3194,6 +4564,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3214,6 +4594,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3234,6 +4624,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3254,6 +4654,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3274,6 +4684,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3294,6 +4714,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3314,6 +4744,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3334,6 +4774,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3354,6 +4804,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3374,6 +4834,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3394,6 +4864,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3414,6 +4894,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3434,6 +4924,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3454,6 +4954,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3474,6 +4984,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3494,6 +5014,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3514,6 +5044,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3534,6 +5074,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3554,6 +5104,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>6ª</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3574,6 +5134,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3594,6 +5164,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3614,6 +5194,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3634,6 +5224,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3654,6 +5254,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3674,6 +5284,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -3694,6 +5314,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -3714,6 +5344,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3734,6 +5374,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -3754,6 +5404,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -3774,6 +5434,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -3794,6 +5464,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3814,6 +5494,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3834,6 +5524,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3854,6 +5554,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3874,6 +5584,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3894,6 +5614,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3914,6 +5644,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3934,6 +5674,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3954,6 +5704,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3974,6 +5734,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -3994,6 +5764,16 @@
           <t>3ª</t>
         </is>
       </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>3ª</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4014,6 +5794,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4034,6 +5824,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4054,6 +5854,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4074,6 +5884,16 @@
           <t>2ª</t>
         </is>
       </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4094,6 +5914,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4114,6 +5944,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4134,6 +5974,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4154,6 +6004,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4174,6 +6034,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4194,6 +6064,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4214,6 +6094,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>5ª</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4234,6 +6124,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4254,6 +6154,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4274,6 +6184,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4294,6 +6214,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4314,6 +6244,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4334,6 +6274,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4354,6 +6304,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4374,6 +6334,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4394,6 +6364,16 @@
           <t>1ª</t>
         </is>
       </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>2ª</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4414,6 +6394,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4434,6 +6424,16 @@
           <t>Não Alocado</t>
         </is>
       </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Perda</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4452,6 +6452,16 @@
       <c r="D201" t="inlineStr">
         <is>
           <t>2ª</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Perda</t>
         </is>
       </c>
     </row>

</xml_diff>